<commit_message>
committing the trials for the first day of single T maze training
</commit_message>
<xml_diff>
--- a/src/omniroute_operation/src/rule_based_experiment/Training_Trials .xlsx
+++ b/src/omniroute_operation/src/rule_based_experiment/Training_Trials .xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="10">
   <si>
     <t xml:space="preserve">Left_Cue</t>
   </si>
@@ -49,25 +49,6 @@
     <t xml:space="preserve">forced_choice</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">forced_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">choice</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Black</t>
   </si>
 </sst>
@@ -78,7 +59,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -115,28 +96,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -181,7 +145,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -199,18 +163,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -233,11 +185,11 @@
   </sheetPr>
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G55" activeCellId="0" sqref="G55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="11.71"/>
   </cols>
@@ -274,7 +226,7 @@
       </c>
       <c r="E2" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.703728160433975</v>
+        <v>0.325341825288847</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -284,15 +236,15 @@
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>9</v>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.68315721817932</v>
+        <v>0.736949194848838</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -302,69 +254,69 @@
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>9</v>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.91112092037946</v>
+        <v>0.76950926060755</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E5" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.862919104472976</v>
+        <v>0.198476696039102</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E6" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.275609655010023</v>
+        <v>0.572876886956201</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E7" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.193600986261705</v>
+        <v>0.14124046393787</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -374,15 +326,15 @@
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>9</v>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E8" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.388707142039832</v>
+        <v>0.349876633085204</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -395,12 +347,12 @@
       <c r="C9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>9</v>
+      <c r="D9" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E9" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.8898837849441</v>
+        <v>0.859936170081302</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -410,15 +362,15 @@
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>9</v>
+      <c r="C10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E10" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.712689436168145</v>
+        <v>0.0333754070501721</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -428,7 +380,7 @@
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -436,7 +388,7 @@
       </c>
       <c r="E11" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.701103725940792</v>
+        <v>0.210536406038008</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -446,15 +398,15 @@
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>9</v>
+      <c r="C12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E12" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.251746514208332</v>
+        <v>0.817265043890606</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -464,15 +416,15 @@
       <c r="B13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>9</v>
+      <c r="C13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E13" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.00771700734842541</v>
+        <v>0.285758522491754</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -482,15 +434,15 @@
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>9</v>
+      <c r="C14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E14" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.34416299842353</v>
+        <v>0.0380000034580211</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -500,15 +452,15 @@
       <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>9</v>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E15" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.868552508149578</v>
+        <v>0.906227525004015</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -521,12 +473,12 @@
       <c r="C16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>9</v>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E16" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.308681683008814</v>
+        <v>0.32416219018021</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -536,15 +488,15 @@
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>9</v>
+      <c r="C17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E17" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.838049142948817</v>
+        <v>0.805858717578101</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -554,15 +506,15 @@
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>9</v>
+      <c r="C18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E18" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.192813842256341</v>
+        <v>0.561488343663837</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -572,15 +524,15 @@
       <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>9</v>
+      <c r="C19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E19" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.745249043172279</v>
+        <v>0.210259245844799</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -590,7 +542,7 @@
       <c r="B20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -598,7 +550,7 @@
       </c>
       <c r="E20" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.383356475127992</v>
+        <v>0.715537780200506</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -608,15 +560,15 @@
       <c r="B21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>9</v>
+      <c r="C21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E21" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.710068583751356</v>
+        <v>0.679905647113464</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -626,15 +578,15 @@
       <c r="B22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>9</v>
+      <c r="C22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E22" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.613268463156387</v>
+        <v>0.705341658699668</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -647,12 +599,12 @@
       <c r="C23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>9</v>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E23" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.745155270051798</v>
+        <v>0.900037112859407</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -662,69 +614,69 @@
       <c r="B24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>9</v>
+      <c r="C24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E24" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.813425454424158</v>
+        <v>0.738065161912534</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E25" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.955062935602156</v>
+        <v>0.298767366707625</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E26" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.564690361663498</v>
+        <v>0.0248798426137125</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E27" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.775977273888789</v>
+        <v>0.361025096301436</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -734,25 +686,25 @@
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>9</v>
+      <c r="C28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E28" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.652783801005377</v>
+        <v>0.463477879596986</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -760,25 +712,25 @@
       </c>
       <c r="E29" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.657332054405596</v>
+        <v>0.899677576848432</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>9</v>
+      <c r="D30" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E30" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.597892245066648</v>
+        <v>0.17486489363463</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -788,15 +740,15 @@
       <c r="B31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>9</v>
+      <c r="C31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E31" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.754912355426012</v>
+        <v>0.919198393139249</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -806,15 +758,15 @@
       <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>9</v>
+      <c r="C32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E32" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.230800727919324</v>
+        <v>0.932599751045215</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -824,15 +776,15 @@
       <c r="B33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>9</v>
+      <c r="C33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E33" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.99047874057445</v>
+        <v>0.687349431227975</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -842,15 +794,15 @@
       <c r="B34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>9</v>
+      <c r="C34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E34" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0740618163482462</v>
+        <v>0.668866102360497</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -860,15 +812,15 @@
       <c r="B35" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>9</v>
+      <c r="C35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E35" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.556824635690992</v>
+        <v>0.299113711228443</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -878,15 +830,15 @@
       <c r="B36" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>9</v>
+      <c r="C36" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E36" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.670353898028697</v>
+        <v>0.253136182277389</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -896,15 +848,15 @@
       <c r="B37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>9</v>
+      <c r="C37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E37" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.138615125794809</v>
+        <v>0.978108447662928</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -914,15 +866,15 @@
       <c r="B38" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>10</v>
+      <c r="C38" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E38" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.143636887872473</v>
+        <v>0.350758258224709</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -932,15 +884,15 @@
       <c r="B39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>9</v>
+      <c r="C39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E39" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.140349001838553</v>
+        <v>0.530027475603528</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -950,15 +902,15 @@
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>9</v>
+      <c r="C40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E40" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.700154555287471</v>
+        <v>0.0932446401893503</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -968,15 +920,15 @@
       <c r="B41" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>9</v>
+      <c r="C41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E41" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.589976218695945</v>
+        <v>0.00586027250121808</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -986,15 +938,15 @@
       <c r="B42" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>9</v>
+      <c r="C42" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E42" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.628731882530868</v>
+        <v>0.134216457692807</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1004,15 +956,15 @@
       <c r="B43" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>9</v>
+      <c r="C43" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E43" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.323978006194974</v>
+        <v>0.807968323442944</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1022,15 +974,15 @@
       <c r="B44" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C44" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>9</v>
+      <c r="C44" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E44" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.637354861051604</v>
+        <v>0.867169010774887</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1040,15 +992,15 @@
       <c r="B45" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>9</v>
+      <c r="C45" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E45" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.27920794858555</v>
+        <v>0.736377004438553</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1058,51 +1010,51 @@
       <c r="B46" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>9</v>
+      <c r="C46" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E46" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.240721888717913</v>
+        <v>0.0754379602488955</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E47" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.927361098609358</v>
+        <v>0.650459452788075</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E48" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.733983773286755</v>
+        <v>0.907833678001237</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1112,15 +1064,15 @@
       <c r="B49" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C49" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>9</v>
+      <c r="C49" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E49" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.997473521896128</v>
+        <v>0.885722060330212</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1130,15 +1082,15 @@
       <c r="B50" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>9</v>
+      <c r="C50" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E50" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.811673965691375</v>
+        <v>0.78925459966701</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1148,15 +1100,15 @@
       <c r="B51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C51" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>9</v>
+      <c r="C51" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E51" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0191105146953704</v>
+        <v>0.582980643174923</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1166,51 +1118,51 @@
       <c r="B52" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>9</v>
+      <c r="C52" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E52" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.850703835528354</v>
+        <v>0.992398338876803</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E53" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.32723552166557</v>
+        <v>0.224072444476191</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E54" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.517399153460635</v>
+        <v>0.483531593234427</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1220,15 +1172,15 @@
       <c r="B55" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>9</v>
+      <c r="C55" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E55" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.212231267891618</v>
+        <v>0.670818653005099</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1238,15 +1190,15 @@
       <c r="B56" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C56" s="6" t="s">
-        <v>10</v>
+      <c r="C56" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E56" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.254933742034375</v>
+        <v>0.862101870153993</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1256,51 +1208,51 @@
       <c r="B57" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C57" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>9</v>
+      <c r="C57" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E57" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.589140341989797</v>
+        <v>0.289151210477785</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E58" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.949211715670042</v>
+        <v>0.82999433924766</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E59" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.745980665929878</v>
+        <v>0.0394516592915679</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1310,15 +1262,15 @@
       <c r="B60" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C60" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>9</v>
+      <c r="C60" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E60" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.280773708810783</v>
+        <v>0.194328067123851</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1328,89 +1280,89 @@
       <c r="B61" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C61" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>9</v>
+      <c r="C61" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E61" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.61703701506609</v>
+        <v>0.228476942232872</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
-      <c r="C62" s="6"/>
+      <c r="C62" s="4"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2"/>
-      <c r="B63" s="6"/>
+      <c r="B63" s="4"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2"/>
-      <c r="B64" s="6"/>
+      <c r="B64" s="4"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2"/>
-      <c r="B65" s="6"/>
+      <c r="B65" s="4"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="6"/>
+      <c r="A66" s="4"/>
       <c r="B66" s="2"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="6"/>
+      <c r="A67" s="4"/>
       <c r="B67" s="2"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="6"/>
+      <c r="A68" s="4"/>
       <c r="B68" s="2"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2"/>
-      <c r="B69" s="6"/>
+      <c r="B69" s="4"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2"/>
-      <c r="B70" s="6"/>
+      <c r="B70" s="4"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="6"/>
+      <c r="A71" s="4"/>
       <c r="B71" s="2"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2"/>
-      <c r="B72" s="6"/>
+      <c r="B72" s="4"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="6"/>
+      <c r="A73" s="4"/>
       <c r="B73" s="2"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="6"/>
+      <c r="A74" s="4"/>
       <c r="B74" s="2"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2"/>
-      <c r="B75" s="6"/>
+      <c r="B75" s="4"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2"/>
-      <c r="B76" s="6"/>
+      <c r="B76" s="4"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="6"/>
+      <c r="A77" s="4"/>
       <c r="B77" s="2"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="6"/>
+      <c r="A78" s="4"/>
       <c r="B78" s="2"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2"/>
-      <c r="B79" s="6"/>
+      <c r="B79" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
making the interval between the doors opening shorter
</commit_message>
<xml_diff>
--- a/src/omniroute_operation/src/rule_based_experiment/Training_Trials .xlsx
+++ b/src/omniroute_operation/src/rule_based_experiment/Training_Trials .xlsx
@@ -59,7 +59,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -94,6 +94,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -145,7 +151,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -163,6 +169,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -186,10 +196,10 @@
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G55" activeCellId="0" sqref="G55"/>
+      <selection pane="topLeft" activeCell="G44" activeCellId="0" sqref="G44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="11.71"/>
   </cols>
@@ -226,7 +236,7 @@
       </c>
       <c r="E2" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.325341825288847</v>
+        <v>0.273331529193377</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -244,7 +254,7 @@
       </c>
       <c r="E3" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.736949194848838</v>
+        <v>0.178948175228277</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -262,7 +272,7 @@
       </c>
       <c r="E4" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.76950926060755</v>
+        <v>0.644673421926885</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -280,7 +290,7 @@
       </c>
       <c r="E5" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.198476696039102</v>
+        <v>0.890207547315201</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -298,7 +308,7 @@
       </c>
       <c r="E6" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.572876886956201</v>
+        <v>0.359687495460723</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -316,7 +326,7 @@
       </c>
       <c r="E7" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.14124046393787</v>
+        <v>0.994982623523181</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -334,7 +344,7 @@
       </c>
       <c r="E8" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.349876633085204</v>
+        <v>0.0309663030108151</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -352,15 +362,15 @@
       </c>
       <c r="E9" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.859936170081302</v>
+        <v>0.412886233890156</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>6</v>
+      <c r="A10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>7</v>
@@ -370,7 +380,7 @@
       </c>
       <c r="E10" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0333754070501721</v>
+        <v>0.475062272129876</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -388,7 +398,7 @@
       </c>
       <c r="E11" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.210536406038008</v>
+        <v>0.442215227550576</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -406,7 +416,7 @@
       </c>
       <c r="E12" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.817265043890606</v>
+        <v>0.725094102282307</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -424,7 +434,7 @@
       </c>
       <c r="E13" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.285758522491754</v>
+        <v>0.931778257412558</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -442,7 +452,7 @@
       </c>
       <c r="E14" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0380000034580211</v>
+        <v>0.364252668196643</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -460,7 +470,7 @@
       </c>
       <c r="E15" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.906227525004015</v>
+        <v>0.860523275140756</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -478,7 +488,7 @@
       </c>
       <c r="E16" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.32416219018021</v>
+        <v>0.0959961056200826</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -496,7 +506,7 @@
       </c>
       <c r="E17" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.805858717578101</v>
+        <v>0.531829072838361</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -514,7 +524,7 @@
       </c>
       <c r="E18" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.561488343663837</v>
+        <v>0.849745129303271</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -532,7 +542,7 @@
       </c>
       <c r="E19" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.210259245844799</v>
+        <v>0.79357143624902</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -550,7 +560,7 @@
       </c>
       <c r="E20" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.715537780200506</v>
+        <v>0.73865308678276</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,7 +578,7 @@
       </c>
       <c r="E21" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.679905647113464</v>
+        <v>0.677090927386594</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -586,7 +596,7 @@
       </c>
       <c r="E22" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.705341658699668</v>
+        <v>0.179501939796005</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -604,7 +614,7 @@
       </c>
       <c r="E23" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.900037112859407</v>
+        <v>0.878122991456431</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -622,7 +632,7 @@
       </c>
       <c r="E24" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.738065161912534</v>
+        <v>0.772775938492751</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -640,7 +650,7 @@
       </c>
       <c r="E25" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.298767366707625</v>
+        <v>0.17397808306813</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -658,7 +668,7 @@
       </c>
       <c r="E26" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0248798426137125</v>
+        <v>0.271502089702446</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -676,7 +686,7 @@
       </c>
       <c r="E27" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.361025096301436</v>
+        <v>0.349671535876271</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -694,7 +704,7 @@
       </c>
       <c r="E28" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.463477879596986</v>
+        <v>0.0799430725437757</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -712,7 +722,7 @@
       </c>
       <c r="E29" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.899677576848432</v>
+        <v>0.255812878316822</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -730,7 +740,7 @@
       </c>
       <c r="E30" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.17486489363463</v>
+        <v>0.65162189122422</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -748,7 +758,7 @@
       </c>
       <c r="E31" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.919198393139249</v>
+        <v>0.316701042034477</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -758,7 +768,7 @@
       <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -766,7 +776,7 @@
       </c>
       <c r="E32" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.932599751045215</v>
+        <v>0.188606917308184</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -776,7 +786,7 @@
       <c r="B33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -784,7 +794,7 @@
       </c>
       <c r="E33" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.687349431227975</v>
+        <v>0.383141976425509</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -794,7 +804,7 @@
       <c r="B34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -802,7 +812,7 @@
       </c>
       <c r="E34" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.668866102360497</v>
+        <v>0.952718718805863</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -812,7 +822,7 @@
       <c r="B35" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -820,7 +830,7 @@
       </c>
       <c r="E35" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.299113711228443</v>
+        <v>0.36379711000746</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -830,7 +840,7 @@
       <c r="B36" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -838,7 +848,7 @@
       </c>
       <c r="E36" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.253136182277389</v>
+        <v>0.110885989169282</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -848,7 +858,7 @@
       <c r="B37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -856,7 +866,7 @@
       </c>
       <c r="E37" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.978108447662928</v>
+        <v>0.0645691213904611</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,7 +876,7 @@
       <c r="B38" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -874,7 +884,7 @@
       </c>
       <c r="E38" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.350758258224709</v>
+        <v>0.338256706515646</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -884,7 +894,7 @@
       <c r="B39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -892,7 +902,7 @@
       </c>
       <c r="E39" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.530027475603528</v>
+        <v>0.700525923335565</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -902,7 +912,7 @@
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D40" s="1" t="s">
@@ -910,7 +920,7 @@
       </c>
       <c r="E40" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0932446401893503</v>
+        <v>0.0233863689246488</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -920,7 +930,7 @@
       <c r="B41" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -928,7 +938,7 @@
       </c>
       <c r="E41" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.00586027250121808</v>
+        <v>0.0127603168005381</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -938,7 +948,7 @@
       <c r="B42" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -946,7 +956,7 @@
       </c>
       <c r="E42" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.134216457692807</v>
+        <v>0.425514559677078</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -956,7 +966,7 @@
       <c r="B43" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -964,7 +974,7 @@
       </c>
       <c r="E43" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.807968323442944</v>
+        <v>0.935144369740662</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -974,7 +984,7 @@
       <c r="B44" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -982,7 +992,7 @@
       </c>
       <c r="E44" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.867169010774887</v>
+        <v>0.362785410503597</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -992,7 +1002,7 @@
       <c r="B45" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -1000,7 +1010,7 @@
       </c>
       <c r="E45" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.736377004438553</v>
+        <v>0.61084357413076</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1010,7 +1020,7 @@
       <c r="B46" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -1018,7 +1028,7 @@
       </c>
       <c r="E46" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0754379602488955</v>
+        <v>0.197973776477566</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1028,7 +1038,7 @@
       <c r="B47" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -1036,7 +1046,7 @@
       </c>
       <c r="E47" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.650459452788075</v>
+        <v>0.0465839301692226</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1046,7 +1056,7 @@
       <c r="B48" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -1054,7 +1064,7 @@
       </c>
       <c r="E48" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.907833678001237</v>
+        <v>0.471248027914702</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1064,7 +1074,7 @@
       <c r="B49" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -1072,7 +1082,7 @@
       </c>
       <c r="E49" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.885722060330212</v>
+        <v>0.619693842890491</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1082,7 +1092,7 @@
       <c r="B50" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -1090,7 +1100,7 @@
       </c>
       <c r="E50" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.78925459966701</v>
+        <v>0.884899227086222</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1100,7 +1110,7 @@
       <c r="B51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -1108,7 +1118,7 @@
       </c>
       <c r="E51" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.582980643174923</v>
+        <v>0.957412636043475</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1118,7 +1128,7 @@
       <c r="B52" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -1126,7 +1136,7 @@
       </c>
       <c r="E52" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.992398338876803</v>
+        <v>0.513391782812122</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1136,7 +1146,7 @@
       <c r="B53" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -1144,7 +1154,7 @@
       </c>
       <c r="E53" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.224072444476191</v>
+        <v>0.731558239626032</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1154,7 +1164,7 @@
       <c r="B54" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -1162,7 +1172,7 @@
       </c>
       <c r="E54" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.483531593234427</v>
+        <v>0.420867174258336</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1172,7 +1182,7 @@
       <c r="B55" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -1180,7 +1190,7 @@
       </c>
       <c r="E55" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.670818653005099</v>
+        <v>0.0936022042472091</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1190,7 +1200,7 @@
       <c r="B56" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -1198,7 +1208,7 @@
       </c>
       <c r="E56" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.862101870153993</v>
+        <v>0.393916569417215</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1208,7 +1218,7 @@
       <c r="B57" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -1216,7 +1226,7 @@
       </c>
       <c r="E57" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.289151210477785</v>
+        <v>0.652060055689474</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1226,7 +1236,7 @@
       <c r="B58" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -1234,7 +1244,7 @@
       </c>
       <c r="E58" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.82999433924766</v>
+        <v>0.920174638486548</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1244,7 +1254,7 @@
       <c r="B59" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D59" s="1" t="s">
@@ -1252,7 +1262,7 @@
       </c>
       <c r="E59" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0394516592915679</v>
+        <v>0.754781872162373</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1262,7 +1272,7 @@
       <c r="B60" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -1270,7 +1280,7 @@
       </c>
       <c r="E60" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.194328067123851</v>
+        <v>0.751933756281358</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1280,7 +1290,7 @@
       <c r="B61" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -1288,81 +1298,81 @@
       </c>
       <c r="E61" s="1" t="n">
         <f aca="true">RAND()</f>
-        <v>0.228476942232872</v>
+        <v>0.707332112638512</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
-      <c r="C62" s="4"/>
+      <c r="C62" s="5"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2"/>
-      <c r="B63" s="4"/>
+      <c r="B63" s="5"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2"/>
-      <c r="B64" s="4"/>
+      <c r="B64" s="5"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2"/>
-      <c r="B65" s="4"/>
+      <c r="B65" s="5"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="4"/>
+      <c r="A66" s="5"/>
       <c r="B66" s="2"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="4"/>
+      <c r="A67" s="5"/>
       <c r="B67" s="2"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="4"/>
+      <c r="A68" s="5"/>
       <c r="B68" s="2"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2"/>
-      <c r="B69" s="4"/>
+      <c r="B69" s="5"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2"/>
-      <c r="B70" s="4"/>
+      <c r="B70" s="5"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="4"/>
+      <c r="A71" s="5"/>
       <c r="B71" s="2"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2"/>
-      <c r="B72" s="4"/>
+      <c r="B72" s="5"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="4"/>
+      <c r="A73" s="5"/>
       <c r="B73" s="2"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="4"/>
+      <c r="A74" s="5"/>
       <c r="B74" s="2"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2"/>
-      <c r="B75" s="4"/>
+      <c r="B75" s="5"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2"/>
-      <c r="B76" s="4"/>
+      <c r="B76" s="5"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="4"/>
+      <c r="A77" s="5"/>
       <c r="B77" s="2"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="4"/>
+      <c r="A78" s="5"/>
       <c r="B78" s="2"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2"/>
-      <c r="B79" s="4"/>
+      <c r="B79" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>